<commit_message>
Add Hatchability Template generation script and file
- Added `create_hatchability_template.py` to generate the Excel template.
- Generated `Hatchability_Template.xlsx` with "Flock Reference" and "Data" sheets.
- Configured formulas for Hatchability, Clear%, Rotten%, and Flock Age.
- Configured Flock Age formula to follow user logic (Setting Date - 1 day offset).
- Added Stacked Column + Line Combo Chart with TextAxis.
- Chart configuration:
    - Primary Y-Axis (Stacked Column): Hatchable/Fertile %, Clear %, Rotten %.
    - Secondary Y-Axis (Line): Hatchability %.
    - Removed Male Ratio % from the graph as requested.

Co-authored-by: syabiladham20 <255771918+syabiladham20@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Hatchability_Template.xlsx
+++ b/Hatchability_Template.xlsx
@@ -170,7 +170,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Data'!M1</f>
+              <f>'Data'!K1</f>
             </strRef>
           </tx>
           <spPr>
@@ -185,7 +185,7 @@
           </cat>
           <val>
             <numRef>
-              <f>'Data'!$M$2:$M$101</f>
+              <f>'Data'!$K$2:$K$101</f>
             </numRef>
           </val>
         </ser>
@@ -249,7 +249,7 @@
           <order val="3"/>
           <tx>
             <strRef>
-              <f>'Data'!N1</f>
+              <f>'Data'!M1</f>
             </strRef>
           </tx>
           <spPr>
@@ -267,7 +267,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Data'!$N$2:$N$101</f>
+              <f>'Data'!$M$2:$M$101</f>
             </numRef>
           </val>
         </ser>
@@ -316,7 +316,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:t>Percentage</a:t>
+                  <a:t>Egg Composition (%)</a:t>
                 </a:r>
               </a:p>
             </rich>
@@ -342,7 +342,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:t>Male Ratio %</a:t>
+                  <a:t>Hatchability %</a:t>
                 </a:r>
               </a:p>
             </rich>

</xml_diff>